<commit_message>
regenerate the jpa and modifying the tables in db
</commit_message>
<xml_diff>
--- a/docs/tables.xlsx
+++ b/docs/tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t xml:space="preserve">item_description</t>
   </si>
@@ -64,12 +64,6 @@
     <t xml:space="preserve">gener</t>
   </si>
   <si>
-    <t xml:space="preserve">material_categourt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">materail_categoury_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">matrial_type</t>
   </si>
   <si>
@@ -83,6 +77,18 @@
   </si>
   <si>
     <t xml:space="preserve">unit_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gener_materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
   </si>
 </sst>
 </file>
@@ -97,6 +103,7 @@
       <sz val="10"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -169,7 +176,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,6 +191,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -203,19 +214,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A32:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.34375"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3883928571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2678571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.2142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.7901785714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1339285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.90625"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4017857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,33 +335,22 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,13 +363,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,6 +378,31 @@
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
return to last point before changing nameing and jpa controllers
</commit_message>
<xml_diff>
--- a/docs/tables.xlsx
+++ b/docs/tables.xlsx
@@ -64,22 +64,22 @@
     <t xml:space="preserve">gener</t>
   </si>
   <si>
+    <t xml:space="preserve">cate</t>
+  </si>
+  <si>
     <t xml:space="preserve">matrial_type</t>
   </si>
   <si>
     <t xml:space="preserve">item_type_desc</t>
   </si>
   <si>
-    <t xml:space="preserve">UNITS</t>
+    <t xml:space="preserve">units</t>
   </si>
   <si>
     <t xml:space="preserve">unit_id</t>
   </si>
   <si>
     <t xml:space="preserve">unit_desc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gener_materials</t>
   </si>
   <si>
     <t xml:space="preserve">generID</t>
@@ -98,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
@@ -119,6 +119,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFDDDDDD"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -176,7 +183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,6 +193,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -206,6 +217,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -217,7 +288,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A32:A34"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -249,7 +320,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2"/>
@@ -270,7 +341,7 @@
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="2"/>
@@ -281,11 +352,11 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -335,22 +406,25 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,13 +437,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,8 +455,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>19</v>
+      <c r="A24" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>20</v>

</xml_diff>